<commit_message>
Still need to make Blur work on double faced cards Fixed Headers on 11
</commit_message>
<xml_diff>
--- a/RemovalData.xlsx
+++ b/RemovalData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="252">
   <si>
     <t>Name</t>
   </si>
@@ -28,6 +28,54 @@
     <t>Total</t>
   </si>
   <si>
+    <t>The Lost Caverns of Ixalan</t>
+  </si>
+  <si>
+    <t>LCI</t>
+  </si>
+  <si>
+    <t>Wilds of Eldraine</t>
+  </si>
+  <si>
+    <t>WOE</t>
+  </si>
+  <si>
+    <t>March of the Machine: The Aftermath</t>
+  </si>
+  <si>
+    <t>MAT</t>
+  </si>
+  <si>
+    <t>March of the Machine</t>
+  </si>
+  <si>
+    <t>MOM</t>
+  </si>
+  <si>
+    <t>Phyrexia: All Will Be One</t>
+  </si>
+  <si>
+    <t>ONE</t>
+  </si>
+  <si>
+    <t>The Brothers' War</t>
+  </si>
+  <si>
+    <t>BRO</t>
+  </si>
+  <si>
+    <t>Dominaria United</t>
+  </si>
+  <si>
+    <t>DMU</t>
+  </si>
+  <si>
+    <t>Streets of New Capenna</t>
+  </si>
+  <si>
+    <t>SNC</t>
+  </si>
+  <si>
     <t>Kamigawa: Neon Dynasty</t>
   </si>
   <si>
@@ -400,16 +448,16 @@
     <t>PLC</t>
   </si>
   <si>
+    <t>Time Spiral Timeshifted</t>
+  </si>
+  <si>
+    <t>TSB</t>
+  </si>
+  <si>
     <t>Time Spiral</t>
   </si>
   <si>
     <t>TSP</t>
-  </si>
-  <si>
-    <t>Time Spiral Timeshifted</t>
-  </si>
-  <si>
-    <t>TSB</t>
   </si>
   <si>
     <t>Coldsnap</t>
@@ -1053,7 +1101,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D117"/>
+  <dimension ref="A1:D125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1066,6 +1114,12 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
@@ -1075,10 +1129,10 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>282</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1089,10 +1143,10 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D3">
-        <v>268</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1103,10 +1157,10 @@
         <v>9</v>
       </c>
       <c r="C4">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="D4">
-        <v>268</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1117,10 +1171,10 @@
         <v>11</v>
       </c>
       <c r="C5">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="D5">
-        <v>272</v>
+        <v>291</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1131,10 +1185,10 @@
         <v>13</v>
       </c>
       <c r="C6">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D6">
-        <v>276</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1145,10 +1199,10 @@
         <v>15</v>
       </c>
       <c r="C7">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D7">
-        <v>300</v>
+        <v>276</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1159,10 +1213,10 @@
         <v>17</v>
       </c>
       <c r="C8">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D8">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1173,10 +1227,10 @@
         <v>19</v>
       </c>
       <c r="C9">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D9">
-        <v>280</v>
+        <v>305</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1187,10 +1241,10 @@
         <v>21</v>
       </c>
       <c r="C10">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D10">
-        <v>260</v>
+        <v>299</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1201,10 +1255,10 @@
         <v>23</v>
       </c>
       <c r="C11">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D11">
-        <v>268</v>
+        <v>278</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1215,10 +1269,10 @@
         <v>25</v>
       </c>
       <c r="C12">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D12">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1229,10 +1283,10 @@
         <v>27</v>
       </c>
       <c r="C13">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D13">
-        <v>324</v>
+        <v>283</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1243,10 +1297,10 @@
         <v>29</v>
       </c>
       <c r="C14">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D14">
-        <v>261</v>
+        <v>285</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1257,10 +1311,10 @@
         <v>31</v>
       </c>
       <c r="C15">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="D15">
-        <v>263</v>
+        <v>314</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1271,10 +1325,10 @@
         <v>33</v>
       </c>
       <c r="C16">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D16">
-        <v>263</v>
+        <v>281</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1285,10 +1339,10 @@
         <v>35</v>
       </c>
       <c r="C17">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D17">
-        <v>294</v>
+        <v>280</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1299,10 +1353,10 @@
         <v>37</v>
       </c>
       <c r="C18">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="D18">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1313,10 +1367,10 @@
         <v>39</v>
       </c>
       <c r="C19">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D19">
-        <v>200</v>
+        <v>268</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1327,10 +1381,10 @@
         <v>41</v>
       </c>
       <c r="C20">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D20">
-        <v>269</v>
+        <v>282</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1341,10 +1395,10 @@
         <v>43</v>
       </c>
       <c r="C21">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="D21">
-        <v>194</v>
+        <v>324</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1355,10 +1409,10 @@
         <v>45</v>
       </c>
       <c r="C22">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="D22">
-        <v>267</v>
+        <v>261</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1369,10 +1423,10 @@
         <v>47</v>
       </c>
       <c r="C23">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="D23">
-        <v>194</v>
+        <v>263</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1383,10 +1437,10 @@
         <v>49</v>
       </c>
       <c r="C24">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="D24">
-        <v>259</v>
+        <v>263</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1397,10 +1451,10 @@
         <v>51</v>
       </c>
       <c r="C25">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D25">
-        <v>208</v>
+        <v>294</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1411,10 +1465,10 @@
         <v>53</v>
       </c>
       <c r="C26">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D26">
-        <v>282</v>
+        <v>260</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1425,10 +1479,10 @@
         <v>55</v>
       </c>
       <c r="C27">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="D27">
-        <v>182</v>
+        <v>200</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1439,10 +1493,10 @@
         <v>57</v>
       </c>
       <c r="C28">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D28">
-        <v>249</v>
+        <v>269</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1453,10 +1507,10 @@
         <v>59</v>
       </c>
       <c r="C29">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D29">
-        <v>268</v>
+        <v>194</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1467,10 +1521,10 @@
         <v>61</v>
       </c>
       <c r="C30">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D30">
-        <v>249</v>
+        <v>267</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1481,10 +1535,10 @@
         <v>63</v>
       </c>
       <c r="C31">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D31">
-        <v>175</v>
+        <v>194</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1495,10 +1549,10 @@
         <v>65</v>
       </c>
       <c r="C32">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D32">
-        <v>249</v>
+        <v>259</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1509,10 +1563,10 @@
         <v>67</v>
       </c>
       <c r="C33">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D33">
-        <v>264</v>
+        <v>208</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1523,10 +1577,10 @@
         <v>69</v>
       </c>
       <c r="C34">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D34">
-        <v>165</v>
+        <v>282</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1540,7 +1594,7 @@
         <v>27</v>
       </c>
       <c r="D35">
-        <v>165</v>
+        <v>182</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1551,10 +1605,10 @@
         <v>73</v>
       </c>
       <c r="C36">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D36">
-        <v>229</v>
+        <v>249</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1565,10 +1619,10 @@
         <v>75</v>
       </c>
       <c r="C37">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D37">
-        <v>229</v>
+        <v>268</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1579,10 +1633,10 @@
         <v>77</v>
       </c>
       <c r="C38">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="D38">
-        <v>156</v>
+        <v>249</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1593,10 +1647,10 @@
         <v>79</v>
       </c>
       <c r="C39">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D39">
-        <v>249</v>
+        <v>175</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1607,7 +1661,7 @@
         <v>81</v>
       </c>
       <c r="C40">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D40">
         <v>249</v>
@@ -1621,10 +1675,10 @@
         <v>83</v>
       </c>
       <c r="C41">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="D41">
-        <v>229</v>
+        <v>264</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1638,7 +1692,7 @@
         <v>34</v>
       </c>
       <c r="D42">
-        <v>229</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1649,10 +1703,10 @@
         <v>87</v>
       </c>
       <c r="C43">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D43">
-        <v>158</v>
+        <v>165</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1663,10 +1717,10 @@
         <v>89</v>
       </c>
       <c r="C44">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D44">
-        <v>249</v>
+        <v>229</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1677,7 +1731,7 @@
         <v>91</v>
       </c>
       <c r="C45">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D45">
         <v>229</v>
@@ -1691,10 +1745,10 @@
         <v>93</v>
       </c>
       <c r="C46">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D46">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1705,10 +1759,10 @@
         <v>95</v>
       </c>
       <c r="C47">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="D47">
-        <v>145</v>
+        <v>249</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1719,10 +1773,10 @@
         <v>97</v>
       </c>
       <c r="C48">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D48">
-        <v>229</v>
+        <v>249</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1733,7 +1787,7 @@
         <v>99</v>
       </c>
       <c r="C49">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D49">
         <v>229</v>
@@ -1747,10 +1801,10 @@
         <v>101</v>
       </c>
       <c r="C50">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D50">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1761,10 +1815,10 @@
         <v>103</v>
       </c>
       <c r="C51">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D51">
-        <v>145</v>
+        <v>158</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1775,10 +1829,10 @@
         <v>105</v>
       </c>
       <c r="C52">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D52">
-        <v>229</v>
+        <v>249</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1789,7 +1843,7 @@
         <v>107</v>
       </c>
       <c r="C53">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D53">
         <v>229</v>
@@ -1803,10 +1857,10 @@
         <v>109</v>
       </c>
       <c r="C54">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D54">
-        <v>145</v>
+        <v>165</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1817,7 +1871,7 @@
         <v>111</v>
       </c>
       <c r="C55">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D55">
         <v>145</v>
@@ -1831,7 +1885,7 @@
         <v>113</v>
       </c>
       <c r="C56">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D56">
         <v>229</v>
@@ -1845,10 +1899,10 @@
         <v>115</v>
       </c>
       <c r="C57">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D57">
-        <v>180</v>
+        <v>229</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1859,10 +1913,10 @@
         <v>117</v>
       </c>
       <c r="C58">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D58">
-        <v>281</v>
+        <v>228</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1873,10 +1927,10 @@
         <v>119</v>
       </c>
       <c r="C59">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D59">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1887,10 +1941,10 @@
         <v>121</v>
       </c>
       <c r="C60">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D60">
-        <v>281</v>
+        <v>229</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1901,10 +1955,10 @@
         <v>123</v>
       </c>
       <c r="C61">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="D61">
-        <v>363</v>
+        <v>229</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1915,10 +1969,10 @@
         <v>125</v>
       </c>
       <c r="C62">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D62">
-        <v>180</v>
+        <v>145</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1929,10 +1983,10 @@
         <v>127</v>
       </c>
       <c r="C63">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D63">
-        <v>165</v>
+        <v>145</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1943,10 +1997,10 @@
         <v>129</v>
       </c>
       <c r="C64">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="D64">
-        <v>281</v>
+        <v>229</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1960,7 +2014,7 @@
         <v>25</v>
       </c>
       <c r="D65">
-        <v>121</v>
+        <v>180</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1971,10 +2025,10 @@
         <v>133</v>
       </c>
       <c r="C66">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="D66">
-        <v>150</v>
+        <v>281</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -1985,10 +2039,10 @@
         <v>135</v>
       </c>
       <c r="C67">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D67">
-        <v>180</v>
+        <v>150</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1999,10 +2053,10 @@
         <v>137</v>
       </c>
       <c r="C68">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="D68">
-        <v>165</v>
+        <v>281</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -2013,10 +2067,10 @@
         <v>139</v>
       </c>
       <c r="C69">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D69">
-        <v>286</v>
+        <v>363</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -2027,10 +2081,10 @@
         <v>141</v>
       </c>
       <c r="C70">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="D70">
-        <v>339</v>
+        <v>180</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -2041,7 +2095,7 @@
         <v>143</v>
       </c>
       <c r="C71">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D71">
         <v>165</v>
@@ -2055,10 +2109,10 @@
         <v>145</v>
       </c>
       <c r="C72">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D72">
-        <v>165</v>
+        <v>121</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -2069,10 +2123,10 @@
         <v>147</v>
       </c>
       <c r="C73">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D73">
-        <v>286</v>
+        <v>281</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -2083,10 +2137,10 @@
         <v>149</v>
       </c>
       <c r="C74">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D74">
-        <v>165</v>
+        <v>150</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -2097,10 +2151,10 @@
         <v>151</v>
       </c>
       <c r="C75">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D75">
-        <v>165</v>
+        <v>180</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -2111,10 +2165,10 @@
         <v>153</v>
       </c>
       <c r="C76">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="D76">
-        <v>286</v>
+        <v>165</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -2125,10 +2179,10 @@
         <v>155</v>
       </c>
       <c r="C77">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D77">
-        <v>337</v>
+        <v>286</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -2139,10 +2193,10 @@
         <v>157</v>
       </c>
       <c r="C78">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="D78">
-        <v>143</v>
+        <v>339</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -2153,10 +2207,10 @@
         <v>159</v>
       </c>
       <c r="C79">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D79">
-        <v>145</v>
+        <v>165</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -2167,10 +2221,10 @@
         <v>161</v>
       </c>
       <c r="C80">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D80">
-        <v>330</v>
+        <v>165</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -2181,10 +2235,10 @@
         <v>163</v>
       </c>
       <c r="C81">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="D81">
-        <v>143</v>
+        <v>286</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -2195,10 +2249,10 @@
         <v>165</v>
       </c>
       <c r="C82">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D82">
-        <v>143</v>
+        <v>165</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -2209,10 +2263,10 @@
         <v>167</v>
       </c>
       <c r="C83">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="D83">
-        <v>330</v>
+        <v>165</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -2223,10 +2277,10 @@
         <v>169</v>
       </c>
       <c r="C84">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="D84">
-        <v>143</v>
+        <v>286</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -2237,10 +2291,10 @@
         <v>171</v>
       </c>
       <c r="C85">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D85">
-        <v>330</v>
+        <v>337</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -2251,7 +2305,7 @@
         <v>173</v>
       </c>
       <c r="C86">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D86">
         <v>143</v>
@@ -2265,10 +2319,10 @@
         <v>175</v>
       </c>
       <c r="C87">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="D87">
-        <v>330</v>
+        <v>145</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -2279,10 +2333,10 @@
         <v>177</v>
       </c>
       <c r="C88">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="D88">
-        <v>143</v>
+        <v>330</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -2293,7 +2347,7 @@
         <v>179</v>
       </c>
       <c r="C89">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D89">
         <v>143</v>
@@ -2307,10 +2361,10 @@
         <v>181</v>
       </c>
       <c r="C90">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="D90">
-        <v>330</v>
+        <v>143</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -2321,10 +2375,10 @@
         <v>183</v>
       </c>
       <c r="C91">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="D91">
-        <v>143</v>
+        <v>330</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -2335,10 +2389,10 @@
         <v>185</v>
       </c>
       <c r="C92">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D92">
-        <v>330</v>
+        <v>143</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -2349,10 +2403,10 @@
         <v>187</v>
       </c>
       <c r="C93">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="D93">
-        <v>143</v>
+        <v>330</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -2363,10 +2417,10 @@
         <v>189</v>
       </c>
       <c r="C94">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="D94">
-        <v>330</v>
+        <v>143</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -2377,10 +2431,10 @@
         <v>191</v>
       </c>
       <c r="C95">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="D95">
-        <v>143</v>
+        <v>330</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -2391,7 +2445,7 @@
         <v>193</v>
       </c>
       <c r="C96">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D96">
         <v>143</v>
@@ -2405,10 +2459,10 @@
         <v>195</v>
       </c>
       <c r="C97">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="D97">
-        <v>330</v>
+        <v>143</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -2419,10 +2473,10 @@
         <v>197</v>
       </c>
       <c r="C98">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="D98">
-        <v>167</v>
+        <v>330</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -2433,10 +2487,10 @@
         <v>199</v>
       </c>
       <c r="C99">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D99">
-        <v>429</v>
+        <v>143</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -2447,10 +2501,10 @@
         <v>201</v>
       </c>
       <c r="C100">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D100">
-        <v>167</v>
+        <v>330</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -2461,10 +2515,10 @@
         <v>203</v>
       </c>
       <c r="C101">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="D101">
-        <v>330</v>
+        <v>143</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -2475,10 +2529,10 @@
         <v>205</v>
       </c>
       <c r="C102">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="D102">
-        <v>144</v>
+        <v>330</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -2489,10 +2543,10 @@
         <v>207</v>
       </c>
       <c r="C103">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D103">
-        <v>115</v>
+        <v>143</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -2503,10 +2557,10 @@
         <v>209</v>
       </c>
       <c r="C104">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="D104">
-        <v>363</v>
+        <v>143</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -2517,10 +2571,10 @@
         <v>211</v>
       </c>
       <c r="C105">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D105">
-        <v>363</v>
+        <v>330</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -2531,10 +2585,10 @@
         <v>213</v>
       </c>
       <c r="C106">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="D106">
-        <v>363</v>
+        <v>167</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -2545,10 +2599,10 @@
         <v>215</v>
       </c>
       <c r="C107">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="D107">
-        <v>102</v>
+        <v>429</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -2559,10 +2613,10 @@
         <v>217</v>
       </c>
       <c r="C108">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="D108">
-        <v>119</v>
+        <v>167</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -2573,10 +2627,10 @@
         <v>219</v>
       </c>
       <c r="C109">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="D109">
-        <v>291</v>
+        <v>330</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -2587,10 +2641,10 @@
         <v>221</v>
       </c>
       <c r="C110">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D110">
-        <v>310</v>
+        <v>144</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -2601,10 +2655,10 @@
         <v>223</v>
       </c>
       <c r="C111">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="D111">
-        <v>291</v>
+        <v>115</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -2615,10 +2669,10 @@
         <v>225</v>
       </c>
       <c r="C112">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="D112">
-        <v>291</v>
+        <v>363</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -2629,10 +2683,10 @@
         <v>227</v>
       </c>
       <c r="C113">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="D113">
-        <v>85</v>
+        <v>363</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -2643,10 +2697,10 @@
         <v>229</v>
       </c>
       <c r="C114">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="D114">
-        <v>77</v>
+        <v>363</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -2657,10 +2711,10 @@
         <v>231</v>
       </c>
       <c r="C115">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="D115">
-        <v>287</v>
+        <v>102</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -2671,10 +2725,10 @@
         <v>233</v>
       </c>
       <c r="C116">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="D116">
-        <v>287</v>
+        <v>119</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -2685,9 +2739,121 @@
         <v>235</v>
       </c>
       <c r="C117">
+        <v>30</v>
+      </c>
+      <c r="D117">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" t="s">
+        <v>236</v>
+      </c>
+      <c r="B118" t="s">
+        <v>237</v>
+      </c>
+      <c r="C118">
+        <v>27</v>
+      </c>
+      <c r="D118">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119" t="s">
+        <v>238</v>
+      </c>
+      <c r="B119" t="s">
+        <v>239</v>
+      </c>
+      <c r="C119">
+        <v>30</v>
+      </c>
+      <c r="D119">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120" t="s">
+        <v>240</v>
+      </c>
+      <c r="B120" t="s">
+        <v>241</v>
+      </c>
+      <c r="C120">
+        <v>30</v>
+      </c>
+      <c r="D120">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" t="s">
+        <v>242</v>
+      </c>
+      <c r="B121" t="s">
+        <v>243</v>
+      </c>
+      <c r="C121">
+        <v>9</v>
+      </c>
+      <c r="D121">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122" t="s">
+        <v>244</v>
+      </c>
+      <c r="B122" t="s">
+        <v>245</v>
+      </c>
+      <c r="C122">
+        <v>9</v>
+      </c>
+      <c r="D122">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123" t="s">
+        <v>246</v>
+      </c>
+      <c r="B123" t="s">
+        <v>247</v>
+      </c>
+      <c r="C123">
         <v>31</v>
       </c>
-      <c r="D117">
+      <c r="D123">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124" t="s">
+        <v>248</v>
+      </c>
+      <c r="B124" t="s">
+        <v>249</v>
+      </c>
+      <c r="C124">
+        <v>31</v>
+      </c>
+      <c r="D124">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125" t="s">
+        <v>250</v>
+      </c>
+      <c r="B125" t="s">
+        <v>251</v>
+      </c>
+      <c r="C125">
+        <v>31</v>
+      </c>
+      <c r="D125">
         <v>285</v>
       </c>
     </row>

</xml_diff>